<commit_message>
Add/Update Positions.xlsx via API
</commit_message>
<xml_diff>
--- a/Positions.xlsx
+++ b/Positions.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z303"/>
+  <dimension ref="A1:Z304"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19638,6 +19638,54 @@
         <v>3260.916670967524</v>
       </c>
     </row>
+    <row r="304">
+      <c r="A304" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B304" t="n">
+        <v>732.0925332234001</v>
+      </c>
+      <c r="C304" t="n">
+        <v>133.925933479</v>
+      </c>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+      <c r="G304" t="inlineStr"/>
+      <c r="H304" t="inlineStr"/>
+      <c r="I304" t="n">
+        <v>224.396233723</v>
+      </c>
+      <c r="J304" t="inlineStr"/>
+      <c r="K304" t="n">
+        <v>115.085577602433</v>
+      </c>
+      <c r="L304" t="inlineStr"/>
+      <c r="M304" t="inlineStr"/>
+      <c r="N304" t="n">
+        <v>14.50495952192</v>
+      </c>
+      <c r="O304" t="n">
+        <v>1.0688276907</v>
+      </c>
+      <c r="P304" t="inlineStr"/>
+      <c r="Q304" t="n">
+        <v>1.7472e-06</v>
+      </c>
+      <c r="R304" t="inlineStr"/>
+      <c r="S304" t="inlineStr"/>
+      <c r="T304" t="inlineStr"/>
+      <c r="U304" t="n">
+        <v>175.0068968047128</v>
+      </c>
+      <c r="V304" t="inlineStr"/>
+      <c r="W304" t="inlineStr"/>
+      <c r="X304" t="inlineStr"/>
+      <c r="Y304" t="inlineStr"/>
+      <c r="Z304" t="n">
+        <v>3276.521148937614</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>